<commit_message>
Changing formatting of readme.
</commit_message>
<xml_diff>
--- a/Starter_Code/Model Analysis.xlsx
+++ b/Starter_Code/Model Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eli\Desktop\Homework\Deep_Learning\Deep_Learning_Hmwk\Starter_Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD21C715-DFCE-49C0-BD64-E98903AC2CCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71EE054E-D503-442C-8C4C-E350F8C67F03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4670" yWindow="3640" windowWidth="19180" windowHeight="11070" xr2:uid="{4630AF39-979C-4DFD-9377-715B2A1146CD}"/>
+    <workbookView xWindow="17250" yWindow="760" windowWidth="19180" windowHeight="11070" xr2:uid="{4630AF39-979C-4DFD-9377-715B2A1146CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -69,8 +69,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -115,15 +115,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -443,7 +441,7 @@
   <dimension ref="E3:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="F3" sqref="F3:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -650,9 +648,6 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="E18:I18"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>